<commit_message>
modify the xls headers' format
</commit_message>
<xml_diff>
--- a/test/schema/data/gameAdmin1.xlsx
+++ b/test/schema/data/gameAdmin1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10140" yWindow="3100" windowWidth="19340" windowHeight="13420"/>
+    <workbookView xWindow="10200" yWindow="4540" windowWidth="19340" windowHeight="13420"/>
   </bookViews>
   <sheets>
     <sheet name="Scene" sheetId="2" r:id="rId1"/>
@@ -1369,10 +1369,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1420,110 +1420,110 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="G3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="I3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="J3" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="K3" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>101</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" t="s">
-        <v>32</v>
-      </c>
-      <c r="J4" t="s">
-        <v>33</v>
-      </c>
-      <c r="K4" t="s">
-        <v>34</v>
+        <v>52</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>101001</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="11">
+        <v>0</v>
+      </c>
+      <c r="J4" s="11">
+        <v>0</v>
+      </c>
+      <c r="K4" s="11">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>101</v>
@@ -1538,27 +1538,27 @@
         <v>3</v>
       </c>
       <c r="F5">
-        <v>101001</v>
+        <v>101002</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5" s="11">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J5" s="11">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="K5" s="11">
-        <v>0</v>
+        <v>708</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>101</v>
@@ -1567,13 +1567,13 @@
         <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E6">
         <v>3</v>
       </c>
       <c r="F6">
-        <v>101002</v>
+        <v>101003</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -1582,60 +1582,25 @@
         <v>0</v>
       </c>
       <c r="I6" s="11">
-        <v>9</v>
+        <v>389</v>
       </c>
       <c r="J6" s="11">
-        <v>12</v>
+        <v>-9</v>
       </c>
       <c r="K6" s="11">
-        <v>708</v>
+        <v>-1634</v>
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7">
-        <v>3</v>
-      </c>
-      <c r="B7">
-        <v>101</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-      <c r="F7">
-        <v>101003</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7" s="11">
-        <v>389</v>
-      </c>
-      <c r="J7" s="11">
-        <v>-9</v>
-      </c>
-      <c r="K7" s="11">
-        <v>-1634</v>
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
-      <c r="A8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="10:10">
-      <c r="J19" t="s">
+    <row r="18" spans="10:10">
+      <c r="J18" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1654,10 +1619,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1699,107 +1664,107 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="2">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="6">
-        <v>2</v>
-      </c>
-      <c r="H2" s="6">
-        <v>2</v>
-      </c>
-      <c r="I2" s="6">
-        <v>2</v>
+      <c r="A2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>8</v>
+      <c r="A3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="A4">
+        <v>101001</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="1">
+        <v>-10</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
         <v>10</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>5</v>
+      <c r="F4" s="1">
+        <v>-140</v>
+      </c>
+      <c r="G4" s="8">
+        <v>0</v>
+      </c>
+      <c r="H4" s="8">
+        <v>0</v>
+      </c>
+      <c r="I4" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5">
-        <v>101001</v>
+        <v>101002</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C5" s="1">
-        <v>-10</v>
+        <v>25.52</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
       </c>
       <c r="E5" s="1">
-        <v>10</v>
+        <v>715</v>
       </c>
       <c r="F5" s="1">
         <v>-140</v>
@@ -1815,20 +1780,20 @@
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6">
-        <v>101002</v>
-      </c>
-      <c r="B6" t="s">
-        <v>55</v>
+      <c r="A6" s="12">
+        <v>101003</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="C6" s="1">
-        <v>25.52</v>
+        <v>349.2</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
       </c>
       <c r="E6" s="1">
-        <v>715</v>
+        <v>-1513.42</v>
       </c>
       <c r="F6" s="1">
         <v>-140</v>
@@ -1844,36 +1809,7 @@
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="12">
-        <v>101003</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" s="1">
-        <v>349.2</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1">
-        <v>-1513.42</v>
-      </c>
-      <c r="F7" s="1">
-        <v>-140</v>
-      </c>
-      <c r="G7" s="8">
-        <v>0</v>
-      </c>
-      <c r="H7" s="8">
-        <v>0</v>
-      </c>
-      <c r="I7" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
+      <c r="A7" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>